<commit_message>
Completed implementing data-driven testing using Dataprovider
Need to modify some test steps if use dataprovider
</commit_message>
<xml_diff>
--- a/src/main/resources/TestCaseReference.xlsx
+++ b/src/main/resources/TestCaseReference.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Demo" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Login Success Data" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Login Unsuccess Data" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="OrderProductInChrome-tc01" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Login-tc03" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Login-tc02" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Login-tc01" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="349">
   <si>
     <t xml:space="preserve">Test ID</t>
   </si>
@@ -1054,13 +1055,7 @@
     <t xml:space="preserve">Combo 2 Nước Tẩy Trang Bí Đao Cocoon Làm Sạch &amp; Giảm Dầu 500ml</t>
   </si>
   <si>
-    <t xml:space="preserve">Trang Điểm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trang Điểm Mặt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phấn Phủ Carslan Dạng Nén Vỏ Đen Màu Tím 8g</t>
+    <t xml:space="preserve">Nước Tẩy Trang L'Oreal Tươi Mát Cho Da Dầu, Hỗn Hợp 400ml</t>
   </si>
   <si>
     <t xml:space="preserve">Username</t>
@@ -1069,34 +1064,13 @@
     <t xml:space="preserve">Password</t>
   </si>
   <si>
-    <t xml:space="preserve">Expected Result</t>
-  </si>
-  <si>
     <t xml:space="preserve">0345864246</t>
   </si>
   <si>
     <t xml:space="preserve">#Onimusha00</t>
   </si>
   <si>
-    <t xml:space="preserve">Dat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0796280280</t>
-  </si>
-  <si>
-    <t xml:space="preserve">270519933Phuong</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phương</t>
-  </si>
-  <si>
     <t xml:space="preserve">03458642466</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">07962802800</t>
   </si>
 </sst>
 </file>
@@ -1194,7 +1168,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1217,10 +1191,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -3352,8 +3322,8 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3372,7 +3342,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>340</v>
       </c>
@@ -3385,13 +3355,13 @@
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>343</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>345</v>
       </c>
     </row>
   </sheetData>
@@ -3410,52 +3380,51 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:B1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="1" width="15.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="3" style="1" width="15.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>354</v>
-      </c>
-    </row>
+    </row>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -3472,50 +3441,78 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="3" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.67"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>347</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>356</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix E2E test case Order_One_Product that can run you data driven testing
Begin implement E2E test case Order >2 products
</commit_message>
<xml_diff>
--- a/src/main/resources/TestCaseReference.xlsx
+++ b/src/main/resources/TestCaseReference.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Training\Automation-Testing\src\main\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF3CBB27-6508-4BEC-A0DF-322EB4868580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="OrderProductInChrome-tc01" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Login-tc03" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Login-tc02" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Login-tc01" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="OrderProductInChrome-tc01" sheetId="2" r:id="rId2"/>
+    <sheet name="Login-tc03" sheetId="3" r:id="rId3"/>
+    <sheet name="Login-tc02" sheetId="4" r:id="rId4"/>
+    <sheet name="Login-tc01" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -24,1063 +29,1081 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="349">
-  <si>
-    <t xml:space="preserve">Test ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Module</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Case Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Priority</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Authentication</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User Registration - Valid Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test user registration with valid email and password combinations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">High</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Functional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User Registration - Duplicate Email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test handling of duplicate email registration attempts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Password Strength Validation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test password strength requirements and validation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medium</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Email Verification Process</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test email verification workflow after registration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User Login - Valid Credentials</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test successful login with valid username and password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User Login - Invalid Credentials</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test login failure with incorrect credentials</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Account Lockout</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test account lockout after multiple failed login attempts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Security</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Remember Me Functionality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test persistent login with 'Remember Me' option</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Social Media Login</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test login integration with social media platforms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Integration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Password Reset - Email Delivery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test password reset email delivery and functionality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Password Reset - Link Expiration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test password reset link expiration handling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Account Management</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Profile Information Update</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test updating personal information in user profile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Password Change</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test changing password from user profile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Profile Picture Upload</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test uploading and updating profile picture</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Low</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Address Management</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test adding, editing, and deleting shipping/billing addresses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Product Catalog</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Product Image Display</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test product image loading and display functionality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Image Zoom Functionality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test product image zoom and pan features</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Product Description Display</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test display of product descriptions and details</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ingredient List Display</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test display of cosmetic product ingredient information</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Color/Shade Variations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test display and selection of product color/shade options</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Search</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Keyword Search</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test product search using keywords</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Search Filters - Brand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test filtering search results by brand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Search Filters - Price Range</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test filtering search results by price range</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Search Filters - Product Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test filtering search results by product category/type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Search Filters - Skin Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test filtering cosmetics by skin type compatibility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Search Results Sorting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test sorting search results by price, popularity, ratings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC027</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Navigation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Category Navigation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test browsing products by category (foundation, lipstick, skincare)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC028</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brand Filtering</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test filtering products by specific brands</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC029</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Seasonal Collections</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test navigation and display of seasonal product collections</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC030</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recommendations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Related Products</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test 'You might also like' product recommendations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC031</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recently Viewed Items</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test display of recently viewed products</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC032</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trending Products</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test display of trending/popular products</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC033</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shopping Cart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add Single Item to Cart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test adding individual products to shopping cart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC034</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quantity Selection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test selecting product quantities when adding to cart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC035</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Variant Selection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test selecting product variants (shade, size) when adding to cart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC036</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inventory Availability Check</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test stock availability validation when adding items to cart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC037</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Update Cart Quantities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test updating item quantities in shopping cart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC038</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Remove Cart Items</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test removing items from shopping cart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC039</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Save for Later</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test moving items from cart to saved/wishlist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC040</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cart Persistence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test cart contents persistence across user sessions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC041</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Checkout</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Guest Checkout</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test checkout process without user registration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC042</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shipping Method Selection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test selection of different shipping options</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC043</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tax Calculations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test automatic tax calculation based on location</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC044</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Promo Code Application</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test applying discount/promo codes during checkout</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC045</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Payment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Credit Card Payment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test payment processing with credit/debit cards</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC046</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PayPal Payment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test payment processing through PayPal integration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC047</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Digital Wallet Payment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test payment through digital wallets (Apple Pay, Google Pay)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC048</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Payment Validation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test payment information validation and error handling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC049</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Secure Transaction Processing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test secure payment transaction handling and encryption</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC050</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inventory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Out of Stock Notifications</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test display of out-of-stock product notifications</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC051</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Low Inventory Warnings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test display of low stock warnings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC052</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Backorder Handling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test handling of backordered products</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC053</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Product Info</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Color/Shade Selection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test selection of different product colors and shades</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC054</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Size Options</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test selection of different product sizes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC055</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Limited Edition Availability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test handling of limited edition product availability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC056</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ingredient Information</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test display of detailed ingredient lists</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC057</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Usage Instructions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test display of product usage instructions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC058</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Expiration Date Display</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test display of product expiration dates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC059</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cruelty-Free/Vegan Indicators</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test display of ethical product indicators</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC060</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wishlist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add Items to Wishlist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test adding products to user wishlist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC061</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Remove Items from Wishlist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test removing products from user wishlist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC062</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Share Wishlist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test sharing wishlist with others</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC063</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Move Wishlist Items to Cart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test moving items from wishlist to shopping cart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC064</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reviews</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Submit Product Reviews</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test submitting product reviews and ratings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC065</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Upload Review Photos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test uploading photos with product reviews</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC066</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verified Purchase Indicators</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test display of verified purchase badges on reviews</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC067</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Review Helpfulness Voting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test voting on review helpfulness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC068</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Virtual Try-On</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AR Camera Integration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test augmented reality camera integration for makeup testing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC069</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shade Matching Tools</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test automated shade matching functionality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC070</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Personalization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Skin Tone Quiz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test skin tone assessment quiz functionality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC071</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Personalized Recommendations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test personalized product recommendations based on user profile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC072</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mobile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Touch Interface</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test touch gestures and mobile-optimized interface</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UI/UX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC073</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Swipe Gestures</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test swipe functionality for product images</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC074</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mobile Checkout</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test mobile-optimized checkout process</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC075</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Touch-Friendly Buttons</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test button sizes and touch targets on mobile devices</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC076</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Performance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mobile Loading Speed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test page loading performance on mobile networks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC077</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Image Optimization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test image compression and optimization for mobile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC078</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Offline Browsing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test offline capability for product browsing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC079</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Secure Payment Processing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test payment security and encryption</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC080</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Personal Information Encryption</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test encryption of personal user data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC081</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Privacy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GDPR Compliance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test GDPR compliance features and data handling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Compliance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC082</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Session Management</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test secure session handling and automatic logout</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC083</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XSS Prevention</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test cross-site scripting prevention measures</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC084</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Page Load Speed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test page loading speed optimization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC085</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Image Compression</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test image file compression and optimization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC086</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CDN Performance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test content delivery network performance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC087</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accessibility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Screen Reader Compatibility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test compatibility with screen reader software</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC088</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Keyboard Navigation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test navigation using keyboard only</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC089</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Color Contrast</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test color contrast for visually impaired users</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC090</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Compatibility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cross-Browser Testing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test functionality across different browsers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC091</t>
-  </si>
-  <si>
-    <t xml:space="preserve">browser Version Compatibility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test compatibility with different browser versions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC092</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Admin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inventory Management</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test admin stock level updates and management</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC093</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Product Addition/Removal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test admin ability to add/remove products</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC094</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pricing Changes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test admin price update functionality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC095</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Order Processing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test admin order management and processing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC096</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shipping Updates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test admin shipping status update functionality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC097</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Return Handling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test admin return and refund processing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC098</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Analytics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sales Reporting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test sales report generation and accuracy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reporting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC099</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User Behavior Tracking</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test user behavior analytics and tracking</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conversion Rate Monitoring</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test conversion rate tracking and reporting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Category Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Product Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Product Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chăm Sóc Da Mặt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tẩy Trang Mặt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Combo 2 Nước Tẩy Trang Bí Đao Cocoon Làm Sạch &amp; Giảm Dầu 500ml</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nước Tẩy Trang L'Oreal Tươi Mát Cho Da Dầu, Hỗn Hợp 400ml</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Username</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0345864246</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#Onimusha00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">03458642466</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="356">
+  <si>
+    <t>Test ID</t>
+  </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t>Test Case Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Test Type</t>
+  </si>
+  <si>
+    <t>TC001</t>
+  </si>
+  <si>
+    <t>Authentication</t>
+  </si>
+  <si>
+    <t>User Registration - Valid Data</t>
+  </si>
+  <si>
+    <t>Test user registration with valid email and password combinations</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Functional</t>
+  </si>
+  <si>
+    <t>TC002</t>
+  </si>
+  <si>
+    <t>User Registration - Duplicate Email</t>
+  </si>
+  <si>
+    <t>Test handling of duplicate email registration attempts</t>
+  </si>
+  <si>
+    <t>TC003</t>
+  </si>
+  <si>
+    <t>Password Strength Validation</t>
+  </si>
+  <si>
+    <t>Test password strength requirements and validation</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>TC004</t>
+  </si>
+  <si>
+    <t>Email Verification Process</t>
+  </si>
+  <si>
+    <t>Test email verification workflow after registration</t>
+  </si>
+  <si>
+    <t>TC005</t>
+  </si>
+  <si>
+    <t>User Login - Valid Credentials</t>
+  </si>
+  <si>
+    <t>Test successful login with valid username and password</t>
+  </si>
+  <si>
+    <t>TC006</t>
+  </si>
+  <si>
+    <t>User Login - Invalid Credentials</t>
+  </si>
+  <si>
+    <t>Test login failure with incorrect credentials</t>
+  </si>
+  <si>
+    <t>TC007</t>
+  </si>
+  <si>
+    <t>Account Lockout</t>
+  </si>
+  <si>
+    <t>Test account lockout after multiple failed login attempts</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>TC008</t>
+  </si>
+  <si>
+    <t>Remember Me Functionality</t>
+  </si>
+  <si>
+    <t>Test persistent login with 'Remember Me' option</t>
+  </si>
+  <si>
+    <t>TC009</t>
+  </si>
+  <si>
+    <t>Social Media Login</t>
+  </si>
+  <si>
+    <t>Test login integration with social media platforms</t>
+  </si>
+  <si>
+    <t>Integration</t>
+  </si>
+  <si>
+    <t>TC010</t>
+  </si>
+  <si>
+    <t>Password Reset - Email Delivery</t>
+  </si>
+  <si>
+    <t>Test password reset email delivery and functionality</t>
+  </si>
+  <si>
+    <t>TC011</t>
+  </si>
+  <si>
+    <t>Password Reset - Link Expiration</t>
+  </si>
+  <si>
+    <t>Test password reset link expiration handling</t>
+  </si>
+  <si>
+    <t>TC012</t>
+  </si>
+  <si>
+    <t>Account Management</t>
+  </si>
+  <si>
+    <t>Profile Information Update</t>
+  </si>
+  <si>
+    <t>Test updating personal information in user profile</t>
+  </si>
+  <si>
+    <t>TC013</t>
+  </si>
+  <si>
+    <t>Password Change</t>
+  </si>
+  <si>
+    <t>Test changing password from user profile</t>
+  </si>
+  <si>
+    <t>TC014</t>
+  </si>
+  <si>
+    <t>Profile Picture Upload</t>
+  </si>
+  <si>
+    <t>Test uploading and updating profile picture</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>TC015</t>
+  </si>
+  <si>
+    <t>Address Management</t>
+  </si>
+  <si>
+    <t>Test adding, editing, and deleting shipping/billing addresses</t>
+  </si>
+  <si>
+    <t>TC016</t>
+  </si>
+  <si>
+    <t>Product Catalog</t>
+  </si>
+  <si>
+    <t>Product Image Display</t>
+  </si>
+  <si>
+    <t>Test product image loading and display functionality</t>
+  </si>
+  <si>
+    <t>TC017</t>
+  </si>
+  <si>
+    <t>Image Zoom Functionality</t>
+  </si>
+  <si>
+    <t>Test product image zoom and pan features</t>
+  </si>
+  <si>
+    <t>TC018</t>
+  </si>
+  <si>
+    <t>Product Description Display</t>
+  </si>
+  <si>
+    <t>Test display of product descriptions and details</t>
+  </si>
+  <si>
+    <t>TC019</t>
+  </si>
+  <si>
+    <t>Ingredient List Display</t>
+  </si>
+  <si>
+    <t>Test display of cosmetic product ingredient information</t>
+  </si>
+  <si>
+    <t>TC020</t>
+  </si>
+  <si>
+    <t>Color/Shade Variations</t>
+  </si>
+  <si>
+    <t>Test display and selection of product color/shade options</t>
+  </si>
+  <si>
+    <t>TC021</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>Keyword Search</t>
+  </si>
+  <si>
+    <t>Test product search using keywords</t>
+  </si>
+  <si>
+    <t>TC022</t>
+  </si>
+  <si>
+    <t>Search Filters - Brand</t>
+  </si>
+  <si>
+    <t>Test filtering search results by brand</t>
+  </si>
+  <si>
+    <t>TC023</t>
+  </si>
+  <si>
+    <t>Search Filters - Price Range</t>
+  </si>
+  <si>
+    <t>Test filtering search results by price range</t>
+  </si>
+  <si>
+    <t>TC024</t>
+  </si>
+  <si>
+    <t>Search Filters - Product Type</t>
+  </si>
+  <si>
+    <t>Test filtering search results by product category/type</t>
+  </si>
+  <si>
+    <t>TC025</t>
+  </si>
+  <si>
+    <t>Search Filters - Skin Type</t>
+  </si>
+  <si>
+    <t>Test filtering cosmetics by skin type compatibility</t>
+  </si>
+  <si>
+    <t>TC026</t>
+  </si>
+  <si>
+    <t>Search Results Sorting</t>
+  </si>
+  <si>
+    <t>Test sorting search results by price, popularity, ratings</t>
+  </si>
+  <si>
+    <t>TC027</t>
+  </si>
+  <si>
+    <t>Navigation</t>
+  </si>
+  <si>
+    <t>Category Navigation</t>
+  </si>
+  <si>
+    <t>Test browsing products by category (foundation, lipstick, skincare)</t>
+  </si>
+  <si>
+    <t>TC028</t>
+  </si>
+  <si>
+    <t>Brand Filtering</t>
+  </si>
+  <si>
+    <t>Test filtering products by specific brands</t>
+  </si>
+  <si>
+    <t>TC029</t>
+  </si>
+  <si>
+    <t>Seasonal Collections</t>
+  </si>
+  <si>
+    <t>Test navigation and display of seasonal product collections</t>
+  </si>
+  <si>
+    <t>TC030</t>
+  </si>
+  <si>
+    <t>Recommendations</t>
+  </si>
+  <si>
+    <t>Related Products</t>
+  </si>
+  <si>
+    <t>Test 'You might also like' product recommendations</t>
+  </si>
+  <si>
+    <t>TC031</t>
+  </si>
+  <si>
+    <t>Recently Viewed Items</t>
+  </si>
+  <si>
+    <t>Test display of recently viewed products</t>
+  </si>
+  <si>
+    <t>TC032</t>
+  </si>
+  <si>
+    <t>Trending Products</t>
+  </si>
+  <si>
+    <t>Test display of trending/popular products</t>
+  </si>
+  <si>
+    <t>TC033</t>
+  </si>
+  <si>
+    <t>Shopping Cart</t>
+  </si>
+  <si>
+    <t>Add Single Item to Cart</t>
+  </si>
+  <si>
+    <t>Test adding individual products to shopping cart</t>
+  </si>
+  <si>
+    <t>TC034</t>
+  </si>
+  <si>
+    <t>Quantity Selection</t>
+  </si>
+  <si>
+    <t>Test selecting product quantities when adding to cart</t>
+  </si>
+  <si>
+    <t>TC035</t>
+  </si>
+  <si>
+    <t>Variant Selection</t>
+  </si>
+  <si>
+    <t>Test selecting product variants (shade, size) when adding to cart</t>
+  </si>
+  <si>
+    <t>TC036</t>
+  </si>
+  <si>
+    <t>Inventory Availability Check</t>
+  </si>
+  <si>
+    <t>Test stock availability validation when adding items to cart</t>
+  </si>
+  <si>
+    <t>TC037</t>
+  </si>
+  <si>
+    <t>Update Cart Quantities</t>
+  </si>
+  <si>
+    <t>Test updating item quantities in shopping cart</t>
+  </si>
+  <si>
+    <t>TC038</t>
+  </si>
+  <si>
+    <t>Remove Cart Items</t>
+  </si>
+  <si>
+    <t>Test removing items from shopping cart</t>
+  </si>
+  <si>
+    <t>TC039</t>
+  </si>
+  <si>
+    <t>Save for Later</t>
+  </si>
+  <si>
+    <t>Test moving items from cart to saved/wishlist</t>
+  </si>
+  <si>
+    <t>TC040</t>
+  </si>
+  <si>
+    <t>Cart Persistence</t>
+  </si>
+  <si>
+    <t>Test cart contents persistence across user sessions</t>
+  </si>
+  <si>
+    <t>TC041</t>
+  </si>
+  <si>
+    <t>Checkout</t>
+  </si>
+  <si>
+    <t>Guest Checkout</t>
+  </si>
+  <si>
+    <t>Test checkout process without user registration</t>
+  </si>
+  <si>
+    <t>TC042</t>
+  </si>
+  <si>
+    <t>Shipping Method Selection</t>
+  </si>
+  <si>
+    <t>Test selection of different shipping options</t>
+  </si>
+  <si>
+    <t>TC043</t>
+  </si>
+  <si>
+    <t>Tax Calculations</t>
+  </si>
+  <si>
+    <t>Test automatic tax calculation based on location</t>
+  </si>
+  <si>
+    <t>TC044</t>
+  </si>
+  <si>
+    <t>Promo Code Application</t>
+  </si>
+  <si>
+    <t>Test applying discount/promo codes during checkout</t>
+  </si>
+  <si>
+    <t>TC045</t>
+  </si>
+  <si>
+    <t>Payment</t>
+  </si>
+  <si>
+    <t>Credit Card Payment</t>
+  </si>
+  <si>
+    <t>Test payment processing with credit/debit cards</t>
+  </si>
+  <si>
+    <t>TC046</t>
+  </si>
+  <si>
+    <t>PayPal Payment</t>
+  </si>
+  <si>
+    <t>Test payment processing through PayPal integration</t>
+  </si>
+  <si>
+    <t>TC047</t>
+  </si>
+  <si>
+    <t>Digital Wallet Payment</t>
+  </si>
+  <si>
+    <t>Test payment through digital wallets (Apple Pay, Google Pay)</t>
+  </si>
+  <si>
+    <t>TC048</t>
+  </si>
+  <si>
+    <t>Payment Validation</t>
+  </si>
+  <si>
+    <t>Test payment information validation and error handling</t>
+  </si>
+  <si>
+    <t>TC049</t>
+  </si>
+  <si>
+    <t>Secure Transaction Processing</t>
+  </si>
+  <si>
+    <t>Test secure payment transaction handling and encryption</t>
+  </si>
+  <si>
+    <t>TC050</t>
+  </si>
+  <si>
+    <t>Inventory</t>
+  </si>
+  <si>
+    <t>Out of Stock Notifications</t>
+  </si>
+  <si>
+    <t>Test display of out-of-stock product notifications</t>
+  </si>
+  <si>
+    <t>TC051</t>
+  </si>
+  <si>
+    <t>Low Inventory Warnings</t>
+  </si>
+  <si>
+    <t>Test display of low stock warnings</t>
+  </si>
+  <si>
+    <t>TC052</t>
+  </si>
+  <si>
+    <t>Backorder Handling</t>
+  </si>
+  <si>
+    <t>Test handling of backordered products</t>
+  </si>
+  <si>
+    <t>TC053</t>
+  </si>
+  <si>
+    <t>Product Info</t>
+  </si>
+  <si>
+    <t>Color/Shade Selection</t>
+  </si>
+  <si>
+    <t>Test selection of different product colors and shades</t>
+  </si>
+  <si>
+    <t>TC054</t>
+  </si>
+  <si>
+    <t>Size Options</t>
+  </si>
+  <si>
+    <t>Test selection of different product sizes</t>
+  </si>
+  <si>
+    <t>TC055</t>
+  </si>
+  <si>
+    <t>Limited Edition Availability</t>
+  </si>
+  <si>
+    <t>Test handling of limited edition product availability</t>
+  </si>
+  <si>
+    <t>TC056</t>
+  </si>
+  <si>
+    <t>Ingredient Information</t>
+  </si>
+  <si>
+    <t>Test display of detailed ingredient lists</t>
+  </si>
+  <si>
+    <t>TC057</t>
+  </si>
+  <si>
+    <t>Usage Instructions</t>
+  </si>
+  <si>
+    <t>Test display of product usage instructions</t>
+  </si>
+  <si>
+    <t>TC058</t>
+  </si>
+  <si>
+    <t>Expiration Date Display</t>
+  </si>
+  <si>
+    <t>Test display of product expiration dates</t>
+  </si>
+  <si>
+    <t>TC059</t>
+  </si>
+  <si>
+    <t>Cruelty-Free/Vegan Indicators</t>
+  </si>
+  <si>
+    <t>Test display of ethical product indicators</t>
+  </si>
+  <si>
+    <t>TC060</t>
+  </si>
+  <si>
+    <t>Wishlist</t>
+  </si>
+  <si>
+    <t>Add Items to Wishlist</t>
+  </si>
+  <si>
+    <t>Test adding products to user wishlist</t>
+  </si>
+  <si>
+    <t>TC061</t>
+  </si>
+  <si>
+    <t>Remove Items from Wishlist</t>
+  </si>
+  <si>
+    <t>Test removing products from user wishlist</t>
+  </si>
+  <si>
+    <t>TC062</t>
+  </si>
+  <si>
+    <t>Share Wishlist</t>
+  </si>
+  <si>
+    <t>Test sharing wishlist with others</t>
+  </si>
+  <si>
+    <t>TC063</t>
+  </si>
+  <si>
+    <t>Move Wishlist Items to Cart</t>
+  </si>
+  <si>
+    <t>Test moving items from wishlist to shopping cart</t>
+  </si>
+  <si>
+    <t>TC064</t>
+  </si>
+  <si>
+    <t>Reviews</t>
+  </si>
+  <si>
+    <t>Submit Product Reviews</t>
+  </si>
+  <si>
+    <t>Test submitting product reviews and ratings</t>
+  </si>
+  <si>
+    <t>TC065</t>
+  </si>
+  <si>
+    <t>Upload Review Photos</t>
+  </si>
+  <si>
+    <t>Test uploading photos with product reviews</t>
+  </si>
+  <si>
+    <t>TC066</t>
+  </si>
+  <si>
+    <t>Verified Purchase Indicators</t>
+  </si>
+  <si>
+    <t>Test display of verified purchase badges on reviews</t>
+  </si>
+  <si>
+    <t>TC067</t>
+  </si>
+  <si>
+    <t>Review Helpfulness Voting</t>
+  </si>
+  <si>
+    <t>Test voting on review helpfulness</t>
+  </si>
+  <si>
+    <t>TC068</t>
+  </si>
+  <si>
+    <t>Virtual Try-On</t>
+  </si>
+  <si>
+    <t>AR Camera Integration</t>
+  </si>
+  <si>
+    <t>Test augmented reality camera integration for makeup testing</t>
+  </si>
+  <si>
+    <t>TC069</t>
+  </si>
+  <si>
+    <t>Shade Matching Tools</t>
+  </si>
+  <si>
+    <t>Test automated shade matching functionality</t>
+  </si>
+  <si>
+    <t>TC070</t>
+  </si>
+  <si>
+    <t>Personalization</t>
+  </si>
+  <si>
+    <t>Skin Tone Quiz</t>
+  </si>
+  <si>
+    <t>Test skin tone assessment quiz functionality</t>
+  </si>
+  <si>
+    <t>TC071</t>
+  </si>
+  <si>
+    <t>Personalized Recommendations</t>
+  </si>
+  <si>
+    <t>Test personalized product recommendations based on user profile</t>
+  </si>
+  <si>
+    <t>TC072</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>Touch Interface</t>
+  </si>
+  <si>
+    <t>Test touch gestures and mobile-optimized interface</t>
+  </si>
+  <si>
+    <t>UI/UX</t>
+  </si>
+  <si>
+    <t>TC073</t>
+  </si>
+  <si>
+    <t>Swipe Gestures</t>
+  </si>
+  <si>
+    <t>Test swipe functionality for product images</t>
+  </si>
+  <si>
+    <t>TC074</t>
+  </si>
+  <si>
+    <t>Mobile Checkout</t>
+  </si>
+  <si>
+    <t>Test mobile-optimized checkout process</t>
+  </si>
+  <si>
+    <t>TC075</t>
+  </si>
+  <si>
+    <t>Touch-Friendly Buttons</t>
+  </si>
+  <si>
+    <t>Test button sizes and touch targets on mobile devices</t>
+  </si>
+  <si>
+    <t>TC076</t>
+  </si>
+  <si>
+    <t>Performance</t>
+  </si>
+  <si>
+    <t>Mobile Loading Speed</t>
+  </si>
+  <si>
+    <t>Test page loading performance on mobile networks</t>
+  </si>
+  <si>
+    <t>TC077</t>
+  </si>
+  <si>
+    <t>Image Optimization</t>
+  </si>
+  <si>
+    <t>Test image compression and optimization for mobile</t>
+  </si>
+  <si>
+    <t>TC078</t>
+  </si>
+  <si>
+    <t>Offline Browsing</t>
+  </si>
+  <si>
+    <t>Test offline capability for product browsing</t>
+  </si>
+  <si>
+    <t>TC079</t>
+  </si>
+  <si>
+    <t>Secure Payment Processing</t>
+  </si>
+  <si>
+    <t>Test payment security and encryption</t>
+  </si>
+  <si>
+    <t>TC080</t>
+  </si>
+  <si>
+    <t>Personal Information Encryption</t>
+  </si>
+  <si>
+    <t>Test encryption of personal user data</t>
+  </si>
+  <si>
+    <t>TC081</t>
+  </si>
+  <si>
+    <t>Privacy</t>
+  </si>
+  <si>
+    <t>GDPR Compliance</t>
+  </si>
+  <si>
+    <t>Test GDPR compliance features and data handling</t>
+  </si>
+  <si>
+    <t>Compliance</t>
+  </si>
+  <si>
+    <t>TC082</t>
+  </si>
+  <si>
+    <t>Session Management</t>
+  </si>
+  <si>
+    <t>Test secure session handling and automatic logout</t>
+  </si>
+  <si>
+    <t>TC083</t>
+  </si>
+  <si>
+    <t>XSS Prevention</t>
+  </si>
+  <si>
+    <t>Test cross-site scripting prevention measures</t>
+  </si>
+  <si>
+    <t>TC084</t>
+  </si>
+  <si>
+    <t>Page Load Speed</t>
+  </si>
+  <si>
+    <t>Test page loading speed optimization</t>
+  </si>
+  <si>
+    <t>TC085</t>
+  </si>
+  <si>
+    <t>Image Compression</t>
+  </si>
+  <si>
+    <t>Test image file compression and optimization</t>
+  </si>
+  <si>
+    <t>TC086</t>
+  </si>
+  <si>
+    <t>CDN Performance</t>
+  </si>
+  <si>
+    <t>Test content delivery network performance</t>
+  </si>
+  <si>
+    <t>TC087</t>
+  </si>
+  <si>
+    <t>Accessibility</t>
+  </si>
+  <si>
+    <t>Screen Reader Compatibility</t>
+  </si>
+  <si>
+    <t>Test compatibility with screen reader software</t>
+  </si>
+  <si>
+    <t>TC088</t>
+  </si>
+  <si>
+    <t>Keyboard Navigation</t>
+  </si>
+  <si>
+    <t>Test navigation using keyboard only</t>
+  </si>
+  <si>
+    <t>TC089</t>
+  </si>
+  <si>
+    <t>Color Contrast</t>
+  </si>
+  <si>
+    <t>Test color contrast for visually impaired users</t>
+  </si>
+  <si>
+    <t>TC090</t>
+  </si>
+  <si>
+    <t>Compatibility</t>
+  </si>
+  <si>
+    <t>Cross-Browser Testing</t>
+  </si>
+  <si>
+    <t>Test functionality across different browsers</t>
+  </si>
+  <si>
+    <t>TC091</t>
+  </si>
+  <si>
+    <t>browser Version Compatibility</t>
+  </si>
+  <si>
+    <t>Test compatibility with different browser versions</t>
+  </si>
+  <si>
+    <t>TC092</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Inventory Management</t>
+  </si>
+  <si>
+    <t>Test admin stock level updates and management</t>
+  </si>
+  <si>
+    <t>TC093</t>
+  </si>
+  <si>
+    <t>Product Addition/Removal</t>
+  </si>
+  <si>
+    <t>Test admin ability to add/remove products</t>
+  </si>
+  <si>
+    <t>TC094</t>
+  </si>
+  <si>
+    <t>Pricing Changes</t>
+  </si>
+  <si>
+    <t>Test admin price update functionality</t>
+  </si>
+  <si>
+    <t>TC095</t>
+  </si>
+  <si>
+    <t>Order Processing</t>
+  </si>
+  <si>
+    <t>Test admin order management and processing</t>
+  </si>
+  <si>
+    <t>TC096</t>
+  </si>
+  <si>
+    <t>Shipping Updates</t>
+  </si>
+  <si>
+    <t>Test admin shipping status update functionality</t>
+  </si>
+  <si>
+    <t>TC097</t>
+  </si>
+  <si>
+    <t>Return Handling</t>
+  </si>
+  <si>
+    <t>Test admin return and refund processing</t>
+  </si>
+  <si>
+    <t>TC098</t>
+  </si>
+  <si>
+    <t>Analytics</t>
+  </si>
+  <si>
+    <t>Sales Reporting</t>
+  </si>
+  <si>
+    <t>Test sales report generation and accuracy</t>
+  </si>
+  <si>
+    <t>Reporting</t>
+  </si>
+  <si>
+    <t>TC099</t>
+  </si>
+  <si>
+    <t>User Behavior Tracking</t>
+  </si>
+  <si>
+    <t>Test user behavior analytics and tracking</t>
+  </si>
+  <si>
+    <t>TC100</t>
+  </si>
+  <si>
+    <t>Conversion Rate Monitoring</t>
+  </si>
+  <si>
+    <t>Test conversion rate tracking and reporting</t>
+  </si>
+  <si>
+    <t>Category Name</t>
+  </si>
+  <si>
+    <t>Product Type</t>
+  </si>
+  <si>
+    <t>Product Name</t>
+  </si>
+  <si>
+    <t>Chăm Sóc Da Mặt</t>
+  </si>
+  <si>
+    <t>Tẩy Trang Mặt</t>
+  </si>
+  <si>
+    <t>Combo 2 Nước Tẩy Trang Bí Đao Cocoon Làm Sạch &amp; Giảm Dầu 500ml</t>
+  </si>
+  <si>
+    <t>Nước Tẩy Trang L'Oreal Tươi Mát Cho Da Dầu, Hỗn Hợp 400ml</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>0345864246</t>
+  </si>
+  <si>
+    <t>#Onimusha00</t>
+  </si>
+  <si>
+    <t>03458642466</t>
+  </si>
+  <si>
+    <t>Chăm Sóc Tóc Và Da Đầu</t>
+  </si>
+  <si>
+    <t>Combo 2 Dầu Gội OGX Biotin &amp; Collagen Làm Dày Tóc 385ml</t>
+  </si>
+  <si>
+    <t>Marc Jacobs</t>
+  </si>
+  <si>
+    <t>Nước Hoa Nữ Marc Jacobs Daisy Love Eau So Sweet EDT 30ml</t>
+  </si>
+  <si>
+    <t>Dầu Gội</t>
+  </si>
+  <si>
+    <t>Expected Quantity In Cart</t>
+  </si>
+  <si>
+    <t>Nước Hoa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1089,22 +1112,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -1118,6 +1126,24 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFE3E3E3"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1128,80 +1154,59 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1260,31 +1265,339 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF2F5597"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:F101"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AMK101"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="47.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="69.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="1" width="47.7"/>
+    <col min="1" max="1" width="17" style="1" customWidth="1"/>
+    <col min="2" max="3" width="47.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="69.7109375" style="1" customWidth="1"/>
+    <col min="5" max="1025" width="47.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1304,7 +1617,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -1324,7 +1637,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -1344,7 +1657,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
@@ -1364,7 +1677,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>19</v>
       </c>
@@ -1384,7 +1697,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>22</v>
       </c>
@@ -1404,7 +1717,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>25</v>
       </c>
@@ -1424,7 +1737,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>28</v>
       </c>
@@ -1444,7 +1757,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>32</v>
       </c>
@@ -1464,7 +1777,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>35</v>
       </c>
@@ -1484,7 +1797,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>39</v>
       </c>
@@ -1504,7 +1817,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>42</v>
       </c>
@@ -1524,7 +1837,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>45</v>
       </c>
@@ -1544,7 +1857,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>49</v>
       </c>
@@ -1564,7 +1877,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>52</v>
       </c>
@@ -1584,7 +1897,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>56</v>
       </c>
@@ -1604,7 +1917,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>59</v>
       </c>
@@ -1624,7 +1937,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>63</v>
       </c>
@@ -1644,7 +1957,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>66</v>
       </c>
@@ -1664,7 +1977,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>69</v>
       </c>
@@ -1684,7 +1997,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>72</v>
       </c>
@@ -1704,7 +2017,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>75</v>
       </c>
@@ -1724,7 +2037,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>79</v>
       </c>
@@ -1744,7 +2057,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>82</v>
       </c>
@@ -1764,7 +2077,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>85</v>
       </c>
@@ -1784,7 +2097,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>88</v>
       </c>
@@ -1804,7 +2117,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>91</v>
       </c>
@@ -1824,7 +2137,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>94</v>
       </c>
@@ -1844,7 +2157,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>98</v>
       </c>
@@ -1864,7 +2177,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>101</v>
       </c>
@@ -1884,7 +2197,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>104</v>
       </c>
@@ -1904,7 +2217,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>108</v>
       </c>
@@ -1924,7 +2237,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>111</v>
       </c>
@@ -1944,7 +2257,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>114</v>
       </c>
@@ -1964,7 +2277,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>118</v>
       </c>
@@ -1984,7 +2297,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>121</v>
       </c>
@@ -2004,7 +2317,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>124</v>
       </c>
@@ -2024,7 +2337,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>127</v>
       </c>
@@ -2044,7 +2357,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>130</v>
       </c>
@@ -2064,7 +2377,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>133</v>
       </c>
@@ -2084,7 +2397,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>136</v>
       </c>
@@ -2104,7 +2417,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>139</v>
       </c>
@@ -2124,7 +2437,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>143</v>
       </c>
@@ -2144,7 +2457,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>146</v>
       </c>
@@ -2164,7 +2477,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>149</v>
       </c>
@@ -2184,7 +2497,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>152</v>
       </c>
@@ -2204,7 +2517,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>156</v>
       </c>
@@ -2224,7 +2537,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="48" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>159</v>
       </c>
@@ -2244,7 +2557,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="49" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>162</v>
       </c>
@@ -2264,7 +2577,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="50" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>165</v>
       </c>
@@ -2284,7 +2597,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>168</v>
       </c>
@@ -2304,7 +2617,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="52" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>172</v>
       </c>
@@ -2324,7 +2637,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="53" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>175</v>
       </c>
@@ -2344,7 +2657,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="54" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>178</v>
       </c>
@@ -2364,7 +2677,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="55" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>182</v>
       </c>
@@ -2384,7 +2697,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="56" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>185</v>
       </c>
@@ -2404,7 +2717,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="57" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>188</v>
       </c>
@@ -2424,7 +2737,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="58" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>191</v>
       </c>
@@ -2444,7 +2757,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="59" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>194</v>
       </c>
@@ -2464,7 +2777,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="60" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>197</v>
       </c>
@@ -2484,7 +2797,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="61" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>200</v>
       </c>
@@ -2504,7 +2817,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="62" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>204</v>
       </c>
@@ -2524,7 +2837,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="63" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>207</v>
       </c>
@@ -2544,7 +2857,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="64" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>210</v>
       </c>
@@ -2564,7 +2877,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="65" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>213</v>
       </c>
@@ -2584,7 +2897,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="66" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>217</v>
       </c>
@@ -2604,7 +2917,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="67" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>220</v>
       </c>
@@ -2624,7 +2937,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="68" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>223</v>
       </c>
@@ -2644,7 +2957,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="69" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>226</v>
       </c>
@@ -2664,7 +2977,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="70" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>230</v>
       </c>
@@ -2684,7 +2997,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="71" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>233</v>
       </c>
@@ -2704,7 +3017,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="72" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>237</v>
       </c>
@@ -2724,7 +3037,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="73" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>240</v>
       </c>
@@ -2744,7 +3057,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="74" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>245</v>
       </c>
@@ -2764,7 +3077,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="75" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>248</v>
       </c>
@@ -2784,7 +3097,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="76" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>251</v>
       </c>
@@ -2804,7 +3117,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="77" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>254</v>
       </c>
@@ -2824,7 +3137,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="78" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>258</v>
       </c>
@@ -2844,7 +3157,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="79" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>261</v>
       </c>
@@ -2864,7 +3177,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="80" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>264</v>
       </c>
@@ -2884,7 +3197,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="81" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>267</v>
       </c>
@@ -2904,7 +3217,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="82" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>270</v>
       </c>
@@ -2924,7 +3237,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="83" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>275</v>
       </c>
@@ -2944,7 +3257,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="84" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>278</v>
       </c>
@@ -2964,7 +3277,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="85" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>281</v>
       </c>
@@ -2984,7 +3297,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="86" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>284</v>
       </c>
@@ -3004,7 +3317,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="87" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>287</v>
       </c>
@@ -3024,7 +3337,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="88" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>290</v>
       </c>
@@ -3044,7 +3357,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="89" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>294</v>
       </c>
@@ -3064,7 +3377,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="90" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>297</v>
       </c>
@@ -3084,7 +3397,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="91" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>300</v>
       </c>
@@ -3104,7 +3417,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="92" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>304</v>
       </c>
@@ -3124,7 +3437,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="93" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>307</v>
       </c>
@@ -3144,7 +3457,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="94" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>311</v>
       </c>
@@ -3164,7 +3477,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="95" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>314</v>
       </c>
@@ -3184,7 +3497,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="96" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>317</v>
       </c>
@@ -3204,7 +3517,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="97" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>320</v>
       </c>
@@ -3224,7 +3537,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="98" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>323</v>
       </c>
@@ -3244,7 +3557,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="99" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
         <v>326</v>
       </c>
@@ -3264,7 +3577,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="100" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>331</v>
       </c>
@@ -3284,7 +3597,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="101" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>334</v>
       </c>
@@ -3305,44 +3618,39 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="44.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="1" width="29.18"/>
+    <col min="1" max="16384" width="44.28515625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>337</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>338</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1" s="5" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>340</v>
       </c>
@@ -3352,8 +3660,11 @@
       <c r="C2" s="5" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D2" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>340</v>
       </c>
@@ -3363,12 +3674,42 @@
       <c r="C3" s="5" t="s">
         <v>343</v>
       </c>
+      <c r="D3" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>350</v>
+      </c>
+      <c r="D4" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>351</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>352</v>
+      </c>
+      <c r="D5" s="5">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -3376,25 +3717,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B1048576"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:AMH2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="3" style="1" width="15.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.52"/>
+    <col min="1" max="1" width="15.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" style="1" customWidth="1"/>
+    <col min="3" max="1022" width="15.140625" style="1" customWidth="1"/>
+    <col min="1023" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>344</v>
       </c>
@@ -3402,7 +3740,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>346</v>
       </c>
@@ -3410,26 +3748,10 @@
         <v>347</v>
       </c>
     </row>
-    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -3437,25 +3759,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="3" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="1023" width="8.7109375" customWidth="1"/>
+    <col min="1024" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>344</v>
       </c>
@@ -3463,7 +3782,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>348</v>
       </c>
@@ -3472,10 +3791,9 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -3483,23 +3801,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.67"/>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="2" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>344</v>
       </c>
@@ -3507,7 +3822,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>346</v>
       </c>
@@ -3516,10 +3831,9 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Fix Extent Report output: Log now is split into separated test cases
</commit_message>
<xml_diff>
--- a/src/main/resources/TestCaseReference.xlsx
+++ b/src/main/resources/TestCaseReference.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Training\Automation-Testing\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF3CBB27-6508-4BEC-A0DF-322EB4868580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C18AE519-7C80-4776-91D9-E6052ED01F4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="355">
   <si>
     <t>Test ID</t>
   </si>
@@ -1084,19 +1084,16 @@
     <t>Combo 2 Dầu Gội OGX Biotin &amp; Collagen Làm Dày Tóc 385ml</t>
   </si>
   <si>
-    <t>Marc Jacobs</t>
-  </si>
-  <si>
-    <t>Nước Hoa Nữ Marc Jacobs Daisy Love Eau So Sweet EDT 30ml</t>
-  </si>
-  <si>
     <t>Dầu Gội</t>
   </si>
   <si>
     <t>Expected Quantity In Cart</t>
   </si>
   <si>
-    <t>Nước Hoa</t>
+    <t>1</t>
+  </si>
+  <si>
+    <t>8</t>
   </si>
 </sst>
 </file>
@@ -1180,7 +1177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1201,6 +1198,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3625,10 +3625,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="44.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3647,7 +3647,7 @@
         <v>339</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3660,8 +3660,8 @@
       <c r="C2" s="5" t="s">
         <v>342</v>
       </c>
-      <c r="D2" s="5">
-        <v>1</v>
+      <c r="D2" s="8" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3674,8 +3674,8 @@
       <c r="C3" s="5" t="s">
         <v>343</v>
       </c>
-      <c r="D3" s="5">
-        <v>1</v>
+      <c r="D3" s="8" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3683,27 +3683,13 @@
         <v>349</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="D4" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>355</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>351</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>352</v>
-      </c>
-      <c r="D5" s="5">
-        <v>2</v>
+      <c r="D4" s="8" t="s">
+        <v>354</v>
       </c>
     </row>
   </sheetData>

</xml_diff>